<commit_message>
Update user constraints for goods truck
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_BAU.xlsx
+++ b/SuppXLS/Scen_TRA_BAU.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_Irish-TIMES-model\TRA_Update\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93CD37B7-D2C2-4BBA-9AEF-A523D1DA3A11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B0E9ED-BA85-46E1-8390-08110E2F534E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -164,7 +164,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="244">
   <si>
     <t>~UC_Sets: R_E: AllRegions</t>
   </si>
@@ -925,6 +925,9 @@
   <si>
     <t>UP</t>
   </si>
+  <si>
+    <t>User constraints for Passenger transport</t>
+  </si>
 </sst>
 </file>
 
@@ -942,7 +945,7 @@
     <numFmt numFmtId="171" formatCode="0.0000%"/>
     <numFmt numFmtId="172" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1090,6 +1093,14 @@
       <color rgb="FF384350"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="14">
@@ -1276,7 +1287,7 @@
     <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1417,6 +1428,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -3005,10 +3017,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A6:AO224"/>
+  <dimension ref="A3:AO224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O85" sqref="O85"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K78" sqref="K78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3022,6 +3034,13 @@
     <col min="30" max="40" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="3" spans="2:41" ht="21" x14ac:dyDescent="0.4">
+      <c r="C3" s="84" t="s">
+        <v>243</v>
+      </c>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+    </row>
     <row r="6" spans="2:41" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>25</v>
@@ -7017,12 +7036,12 @@
       <c r="AN66" s="22"/>
       <c r="AO66" s="22"/>
     </row>
-    <row r="67" spans="3:41" s="15" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="C67" s="69" t="s">
+    <row r="67" spans="3:41" s="15" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="C67" s="84" t="s">
         <v>236</v>
       </c>
       <c r="D67" s="68"/>
-      <c r="E67" s="22"/>
+      <c r="E67" s="84"/>
       <c r="F67" s="22"/>
       <c r="G67" s="22"/>
       <c r="H67" s="22"/>
@@ -7350,7 +7369,7 @@
         <v>2018</v>
       </c>
       <c r="K72" s="15" t="s">
-        <v>242</v>
+        <v>66</v>
       </c>
       <c r="L72" s="22">
         <v>-1</v>
@@ -7482,7 +7501,7 @@
         <v>0</v>
       </c>
       <c r="K73" s="76" t="s">
-        <v>242</v>
+        <v>66</v>
       </c>
       <c r="L73" s="22"/>
       <c r="M73" s="22"/>
@@ -7537,7 +7556,7 @@
         <v>2018</v>
       </c>
       <c r="K74" s="76" t="s">
-        <v>242</v>
+        <v>66</v>
       </c>
       <c r="L74" s="22">
         <v>-1</v>
@@ -7669,7 +7688,7 @@
         <v>0</v>
       </c>
       <c r="K75" s="76" t="s">
-        <v>242</v>
+        <v>66</v>
       </c>
       <c r="L75" s="22"/>
       <c r="M75" s="22"/>
@@ -7911,7 +7930,7 @@
         <v>2018</v>
       </c>
       <c r="K78" s="76" t="s">
-        <v>242</v>
+        <v>66</v>
       </c>
       <c r="L78" s="22">
         <v>-1</v>
@@ -8042,8 +8061,8 @@
       <c r="J79" s="30">
         <v>0</v>
       </c>
-      <c r="K79" s="76" t="s">
-        <v>242</v>
+      <c r="K79" s="20" t="s">
+        <v>66</v>
       </c>
       <c r="L79" s="20"/>
       <c r="M79" s="20"/>

</xml_diff>

<commit_message>
Change UC for Freight Transport
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_BAU.xlsx
+++ b/SuppXLS/Scen_TRA_BAU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B0E9ED-BA85-46E1-8390-08110E2F534E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC760AD-8AD2-42B3-A830-50DE59A206A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -164,7 +164,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="243">
   <si>
     <t>~UC_Sets: R_E: AllRegions</t>
   </si>
@@ -921,9 +921,6 @@
   </si>
   <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>UP</t>
   </si>
   <si>
     <t>User constraints for Passenger transport</t>
@@ -3020,7 +3017,7 @@
   <dimension ref="A3:AO224"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K78" sqref="K78"/>
+      <selection activeCell="J83" sqref="J83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3036,7 +3033,7 @@
   <sheetData>
     <row r="3" spans="2:41" ht="21" x14ac:dyDescent="0.4">
       <c r="C3" s="84" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D3" s="69"/>
       <c r="E3" s="69"/>
@@ -7743,7 +7740,7 @@
         <v>2018</v>
       </c>
       <c r="K76" s="76" t="s">
-        <v>242</v>
+        <v>66</v>
       </c>
       <c r="L76" s="22">
         <v>-1</v>
@@ -7875,7 +7872,7 @@
         <v>0</v>
       </c>
       <c r="K77" s="76" t="s">
-        <v>242</v>
+        <v>66</v>
       </c>
       <c r="L77" s="22"/>
       <c r="M77" s="22"/>

</xml_diff>

<commit_message>
Fix UC for freight transport
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_BAU.xlsx
+++ b/SuppXLS/Scen_TRA_BAU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC760AD-8AD2-42B3-A830-50DE59A206A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C238C85-1365-4394-B0EE-13B42A137336}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -164,7 +164,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="244">
   <si>
     <t>~UC_Sets: R_E: AllRegions</t>
   </si>
@@ -924,6 +924,9 @@
   </si>
   <si>
     <t>User constraints for Passenger transport</t>
+  </si>
+  <si>
+    <t>FX</t>
   </si>
 </sst>
 </file>
@@ -3016,8 +3019,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A3:AO224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J83" sqref="J83"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K79" sqref="K79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7366,7 +7369,7 @@
         <v>2018</v>
       </c>
       <c r="K72" s="15" t="s">
-        <v>66</v>
+        <v>243</v>
       </c>
       <c r="L72" s="22">
         <v>-1</v>
@@ -7498,7 +7501,7 @@
         <v>0</v>
       </c>
       <c r="K73" s="76" t="s">
-        <v>66</v>
+        <v>243</v>
       </c>
       <c r="L73" s="22"/>
       <c r="M73" s="22"/>
@@ -7553,7 +7556,7 @@
         <v>2018</v>
       </c>
       <c r="K74" s="76" t="s">
-        <v>66</v>
+        <v>243</v>
       </c>
       <c r="L74" s="22">
         <v>-1</v>
@@ -7685,7 +7688,7 @@
         <v>0</v>
       </c>
       <c r="K75" s="76" t="s">
-        <v>66</v>
+        <v>243</v>
       </c>
       <c r="L75" s="22"/>
       <c r="M75" s="22"/>
@@ -7740,7 +7743,7 @@
         <v>2018</v>
       </c>
       <c r="K76" s="76" t="s">
-        <v>66</v>
+        <v>243</v>
       </c>
       <c r="L76" s="22">
         <v>-1</v>
@@ -7872,7 +7875,7 @@
         <v>0</v>
       </c>
       <c r="K77" s="76" t="s">
-        <v>66</v>
+        <v>243</v>
       </c>
       <c r="L77" s="22"/>
       <c r="M77" s="22"/>
@@ -7927,7 +7930,7 @@
         <v>2018</v>
       </c>
       <c r="K78" s="76" t="s">
-        <v>66</v>
+        <v>243</v>
       </c>
       <c r="L78" s="22">
         <v>-1</v>
@@ -8059,7 +8062,7 @@
         <v>0</v>
       </c>
       <c r="K79" s="20" t="s">
-        <v>66</v>
+        <v>243</v>
       </c>
       <c r="L79" s="20"/>
       <c r="M79" s="20"/>

</xml_diff>